<commit_message>
changing interface and tests
</commit_message>
<xml_diff>
--- a/queries_results.xlsx
+++ b/queries_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rogerrsn\Documents\chatpgt_kws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2D75BF-42BF-40A5-A429-B3A59771728D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00B90D9-79D5-4FA7-8B78-1B4FAB4C4320}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{E09B936A-38EE-4B4B-B9E2-6E20092DBBC4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="5652" firstSheet="3" activeTab="5" xr2:uid="{E09B936A-38EE-4B4B-B9E2-6E20092DBBC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Approach 1-SQL" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="230">
   <si>
     <t>Consultas</t>
   </si>
@@ -358,9 +358,6 @@
   </si>
   <si>
     <t>What is the host province of the International Energy Agency?</t>
-  </si>
-  <si>
-    <t>Province Organization International Energy Agency</t>
   </si>
   <si>
     <t>International Energy Agency</t>
@@ -784,12 +781,6 @@
     <t>With keywords extracted by chatgpt, KwS answers the percentage of people who are Hindu by ethnic group living in Thailand</t>
   </si>
   <si>
-    <t xml:space="preserve">KwS did not respond correctly to the keywords provided by ChatGPT. </t>
-  </si>
-  <si>
-    <t>ChatGPT answered for himself</t>
-  </si>
-  <si>
     <t>SELECT province_name FROM provinces WHERE area &gt; 1000;</t>
   </si>
   <si>
@@ -844,6 +835,9 @@
   </si>
   <si>
     <t>SELECT country FROM countries ORDER BY area DESC LIMIT 1;</t>
+  </si>
+  <si>
+    <t>Organization International Energy Agency</t>
   </si>
 </sst>
 </file>
@@ -1451,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD86196B-670E-459A-BA29-F3DD952FE4BF}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -1482,13 +1476,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C2" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1496,13 +1490,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C3" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -1510,13 +1504,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C4" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1528,7 +1522,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="70" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="94.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1540,7 +1534,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="91.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1552,7 +1546,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -1564,7 +1558,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1576,7 +1570,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1588,7 +1582,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.3">
@@ -1596,13 +1590,13 @@
         <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C11" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -1610,13 +1604,13 @@
         <v>42</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C12" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1628,7 +1622,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1640,7 +1634,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1652,7 +1646,7 @@
         <v>15</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1664,7 +1658,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1672,13 +1666,13 @@
         <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>226</v>
-      </c>
-      <c r="C17" s="71" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1686,13 +1680,13 @@
         <v>33</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C18" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1704,7 +1698,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
@@ -1716,7 +1710,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="82.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1724,13 +1718,13 @@
         <v>35</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C21" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
@@ -1742,7 +1736,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1750,13 +1744,13 @@
         <v>75</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C23" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1768,7 +1762,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1780,7 +1774,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1788,13 +1782,13 @@
         <v>40</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C26" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.3">
@@ -1806,7 +1800,7 @@
         <v>15</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1818,7 +1812,7 @@
         <v>15</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1879,7 +1873,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="57" t="s">
         <v>11</v>
@@ -1892,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="57" t="s">
         <v>11</v>
@@ -1905,7 +1899,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="57" t="s">
         <v>11</v>
@@ -1918,13 +1912,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="70" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="71" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E5" s="51"/>
     </row>
@@ -1959,7 +1953,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C8" s="57" t="s">
         <v>11</v>
@@ -1972,7 +1966,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C9" s="68" t="s">
         <v>11</v>
@@ -1985,7 +1979,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C10" s="68" t="s">
         <v>11</v>
@@ -1998,7 +1992,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" s="57" t="s">
         <v>11</v>
@@ -2011,7 +2005,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C12" s="57" t="s">
         <v>11</v>
@@ -2026,7 +2020,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C13" s="57" t="s">
         <v>11</v>
@@ -2039,7 +2033,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="57" t="s">
         <v>11</v>
@@ -2052,7 +2046,7 @@
         <v>67</v>
       </c>
       <c r="B15" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C15" s="57" t="s">
         <v>11</v>
@@ -2065,7 +2059,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C16" s="57" t="s">
         <v>11</v>
@@ -2078,7 +2072,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C17" s="57" t="s">
         <v>11</v>
@@ -2091,13 +2085,13 @@
         <v>33</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C18" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E18" s="52"/>
     </row>
@@ -2106,13 +2100,13 @@
         <v>31</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C19" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E19" s="52"/>
     </row>
@@ -2121,7 +2115,7 @@
         <v>70</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C20" s="57" t="s">
         <v>11</v>
@@ -2134,13 +2128,13 @@
         <v>35</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C21" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E21" s="52"/>
     </row>
@@ -2149,13 +2143,13 @@
         <v>97</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>190</v>
-      </c>
-      <c r="C22" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>191</v>
       </c>
       <c r="E22" s="52"/>
     </row>
@@ -2177,13 +2171,13 @@
         <v>73</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C24" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E24" s="53"/>
     </row>
@@ -2192,7 +2186,7 @@
         <v>38</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C25" s="61" t="s">
         <v>15</v>
@@ -2207,7 +2201,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C26" s="58" t="s">
         <v>11</v>
@@ -2220,7 +2214,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C27" s="58" t="s">
         <v>11</v>
@@ -2234,13 +2228,13 @@
         <v>78</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C28" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" s="52"/>
     </row>
@@ -2304,7 +2298,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E39" s="51"/>
     </row>
@@ -2516,10 +2510,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>6</v>
@@ -2530,13 +2524,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="C2" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="E2" s="51"/>
     </row>
@@ -2545,13 +2539,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>116</v>
-      </c>
-      <c r="C3" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>117</v>
       </c>
       <c r="E3" s="51"/>
     </row>
@@ -2560,13 +2554,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>119</v>
       </c>
       <c r="E4" s="51"/>
     </row>
@@ -2575,13 +2569,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="C5" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="E5" s="51"/>
     </row>
@@ -2590,13 +2584,13 @@
         <v>20</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="C6" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="E6" s="51"/>
     </row>
@@ -2605,13 +2599,13 @@
         <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="C7" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="E7" s="51"/>
     </row>
@@ -2620,13 +2614,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>122</v>
-      </c>
-      <c r="C8" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>123</v>
       </c>
       <c r="E8" s="51"/>
     </row>
@@ -2635,7 +2629,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="58" t="s">
         <v>11</v>
@@ -2648,7 +2642,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C10" s="58" t="s">
         <v>11</v>
@@ -2661,13 +2655,13 @@
         <v>41</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C11" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E11" s="52"/>
     </row>
@@ -2676,13 +2670,13 @@
         <v>42</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C12" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" s="51"/>
     </row>
@@ -2691,13 +2685,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E13" s="52"/>
     </row>
@@ -2706,13 +2700,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="C14" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="E14" s="52"/>
     </row>
@@ -2721,13 +2715,13 @@
         <v>67</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="C15" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="E15" s="52"/>
     </row>
@@ -2736,7 +2730,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="57" t="s">
         <v>11</v>
@@ -2749,7 +2743,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="57" t="s">
         <v>11</v>
@@ -2762,7 +2756,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C18" s="57" t="s">
         <v>11</v>
@@ -2775,7 +2769,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="57" t="s">
         <v>11</v>
@@ -2788,13 +2782,13 @@
         <v>70</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" s="52"/>
     </row>
@@ -2803,13 +2797,13 @@
         <v>35</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E21" s="52"/>
     </row>
@@ -2818,13 +2812,13 @@
         <v>97</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>138</v>
-      </c>
-      <c r="C22" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>139</v>
       </c>
       <c r="E22" s="52"/>
     </row>
@@ -2833,7 +2827,7 @@
         <v>75</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" s="58" t="s">
         <v>11</v>
@@ -2846,13 +2840,13 @@
         <v>73</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C24" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E24" s="53"/>
     </row>
@@ -2861,13 +2855,13 @@
         <v>38</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C25" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E25" s="53"/>
     </row>
@@ -2876,7 +2870,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C26" s="58" t="s">
         <v>11</v>
@@ -2889,7 +2883,7 @@
         <v>107</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C27" s="58" t="s">
         <v>11</v>
@@ -2903,7 +2897,7 @@
         <v>78</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" s="58" t="s">
         <v>15</v>
@@ -3166,10 +3160,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>6</v>
@@ -3180,7 +3174,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="58" t="s">
         <v>11</v>
@@ -3192,7 +3186,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C3" s="58" t="s">
         <v>11</v>
@@ -3204,13 +3198,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3218,13 +3212,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="C5" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3232,13 +3226,13 @@
         <v>20</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3246,13 +3240,13 @@
         <v>22</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C7" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3260,13 +3254,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C8" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="37" customFormat="1" x14ac:dyDescent="0.3">
@@ -3274,7 +3268,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" s="58" t="s">
         <v>11</v>
@@ -3286,7 +3280,7 @@
         <v>56</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C10" s="58" t="s">
         <v>11</v>
@@ -3298,7 +3292,7 @@
         <v>41</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="58" t="s">
         <v>11</v>
@@ -3310,7 +3304,7 @@
         <v>42</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C12" s="57" t="s">
         <v>11</v>
@@ -3322,13 +3316,13 @@
         <v>8</v>
       </c>
       <c r="B13" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>156</v>
-      </c>
-      <c r="C13" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="37" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3336,13 +3330,13 @@
         <v>9</v>
       </c>
       <c r="B14" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="C14" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3350,13 +3344,13 @@
         <v>67</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="C15" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3364,7 +3358,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="58" t="s">
         <v>11</v>
@@ -3376,7 +3370,7 @@
         <v>30</v>
       </c>
       <c r="B17" s="42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="58" t="s">
         <v>11</v>
@@ -3388,7 +3382,7 @@
         <v>33</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" s="58" t="s">
         <v>11</v>
@@ -3400,7 +3394,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" s="58" t="s">
         <v>11</v>
@@ -3412,13 +3406,13 @@
         <v>70</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3426,13 +3420,13 @@
         <v>35</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>136</v>
-      </c>
-      <c r="C21" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3440,13 +3434,13 @@
         <v>97</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="24" t="s">
         <v>159</v>
-      </c>
-      <c r="C22" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3454,7 +3448,7 @@
         <v>75</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C23" s="58" t="s">
         <v>11</v>
@@ -3466,13 +3460,13 @@
         <v>73</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="62" t="s">
         <v>141</v>
-      </c>
-      <c r="C24" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="62" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3480,13 +3474,13 @@
         <v>38</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C25" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3494,7 +3488,7 @@
         <v>40</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C26" s="58" t="s">
         <v>11</v>
@@ -3506,13 +3500,13 @@
         <v>107</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C27" s="61" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:4" s="37" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3520,7 +3514,7 @@
         <v>78</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C28" s="58" t="s">
         <v>11</v>
@@ -3552,8 +3546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F89A8B4B-7D4A-4655-B56E-F48DAE930DFA}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3577,7 +3571,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E1" s="31" t="s">
         <v>16</v>
@@ -3639,7 +3633,7 @@
         <v>49</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -3695,7 +3689,7 @@
         <v>52</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3715,7 +3709,7 @@
         <v>54</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -3726,7 +3720,7 @@
         <v>57</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>11</v>
@@ -3753,7 +3747,7 @@
         <v>43</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -3791,7 +3785,7 @@
         <v>59</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -3811,7 +3805,7 @@
         <v>61</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -3939,7 +3933,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3977,7 +3971,7 @@
         <v>43</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -3997,7 +3991,7 @@
         <v>43</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -4059,10 +4053,10 @@
         <v>107</v>
       </c>
       <c r="B27" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>110</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>15</v>
@@ -4071,7 +4065,7 @@
         <v>43</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4091,7 +4085,7 @@
         <v>88</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -4122,8 +4116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A94C91-D6AA-4C28-A6A4-D5D6BAA870BD}">
   <dimension ref="A1:G98"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4147,7 +4141,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>16</v>
@@ -4281,7 +4275,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4292,7 +4286,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>11</v>
@@ -4301,7 +4295,7 @@
         <v>43</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -4357,7 +4351,7 @@
         <v>27</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -4503,7 +4497,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -4540,7 +4534,7 @@
         <v>43</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="37" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4578,7 +4572,7 @@
         <v>72</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4622,19 +4616,19 @@
         <v>107</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>108</v>
+        <v>229</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E27" s="24" t="s">
-        <v>213</v>
+      <c r="E27" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="G27" s="64"/>
     </row>
@@ -4643,7 +4637,7 @@
         <v>78</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C28" s="45" t="s">
         <v>79</v>

</xml_diff>